<commit_message>
Se agrega archivo 01PlantillaPrueba.xlsx, el cual contiene y ya probada plantilla para cargar articulos pasados por Agusto, estos vienen de archivo llamado clasificaciondeproductos.xlsx
</commit_message>
<xml_diff>
--- a/01PlantillaPrueba.xlsx
+++ b/01PlantillaPrueba.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="392">
   <si>
     <t>ItemCode</t>
   </si>
@@ -1200,9 +1203,6 @@
   </si>
   <si>
     <t>TaxCtg</t>
-  </si>
-  <si>
-    <t>11001385069</t>
   </si>
 </sst>
 </file>
@@ -1282,6 +1282,98 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja1 (2)"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="Hoja3"/>
+      <sheetName val="Hoja3 (2)"/>
+      <sheetName val="Hoja3 (3)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>11001385069</v>
+          </cell>
+          <cell r="G2" t="str">
+            <v>TERM PRENS P/VAPOR MACHO 1/4"X5/16"</v>
+          </cell>
+          <cell r="H2" t="str">
+            <v>TERM PRENS P/VAPOR MACHO 1/4"X5/16"</v>
+          </cell>
+          <cell r="I2">
+            <v>110</v>
+          </cell>
+          <cell r="J2" t="str">
+            <v>tYES</v>
+          </cell>
+          <cell r="K2" t="str">
+            <v>tYES</v>
+          </cell>
+          <cell r="L2" t="str">
+            <v>tYES</v>
+          </cell>
+          <cell r="M2" t="str">
+            <v>tYES</v>
+          </cell>
+          <cell r="N2" t="str">
+            <v>NULL</v>
+          </cell>
+          <cell r="O2">
+            <v>0</v>
+          </cell>
+          <cell r="P2" t="str">
+            <v>tNO</v>
+          </cell>
+          <cell r="Q2" t="str">
+            <v>tNO</v>
+          </cell>
+          <cell r="R2" t="str">
+            <v>tNO</v>
+          </cell>
+          <cell r="S2" t="str">
+            <v>UND</v>
+          </cell>
+          <cell r="T2" t="str">
+            <v>UND</v>
+          </cell>
+          <cell r="U2" t="str">
+            <v>W</v>
+          </cell>
+          <cell r="V2">
+            <v>0</v>
+          </cell>
+          <cell r="W2" t="str">
+            <v>tYES</v>
+          </cell>
+          <cell r="X2" t="str">
+            <v>UND</v>
+          </cell>
+          <cell r="Y2">
+            <v>1100</v>
+          </cell>
+          <cell r="Z2">
+            <v>1</v>
+          </cell>
+          <cell r="AA2">
+            <v>38</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1549,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" workbookViewId="0">
-      <selection activeCell="DN1" sqref="DN1:GR1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="GU4" sqref="GU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,7 +1714,7 @@
     <col min="81" max="81" width="16.6328125" hidden="1" customWidth="1"/>
     <col min="82" max="82" width="8.36328125" hidden="1" customWidth="1"/>
     <col min="83" max="83" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="7.7265625" hidden="1" customWidth="1"/>
     <col min="85" max="85" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="87" max="88" width="18.26953125" hidden="1" customWidth="1"/>
@@ -2896,8 +2988,93 @@
       </c>
     </row>
     <row r="3" spans="1:203" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>392</v>
+      <c r="A3" s="2" t="str">
+        <f>+'[1]Hoja3 (3)'!$A$2</f>
+        <v>11001385069</v>
+      </c>
+      <c r="B3" t="str">
+        <f>+'[1]Hoja3 (3)'!$G$2</f>
+        <v>TERM PRENS P/VAPOR MACHO 1/4"X5/16"</v>
+      </c>
+      <c r="C3" t="str">
+        <f>+'[1]Hoja3 (3)'!$H$2</f>
+        <v>TERM PRENS P/VAPOR MACHO 1/4"X5/16"</v>
+      </c>
+      <c r="D3">
+        <f>+'[1]Hoja3 (3)'!$I$2</f>
+        <v>110</v>
+      </c>
+      <c r="H3" t="str">
+        <f>+'[1]Hoja3 (3)'!$J$2</f>
+        <v>tYES</v>
+      </c>
+      <c r="I3" t="str">
+        <f>+'[1]Hoja3 (3)'!$K$2</f>
+        <v>tYES</v>
+      </c>
+      <c r="J3" t="str">
+        <f>+'[1]Hoja3 (3)'!$L$2</f>
+        <v>tYES</v>
+      </c>
+      <c r="K3" t="str">
+        <f>+'[1]Hoja3 (3)'!$M$2</f>
+        <v>tYES</v>
+      </c>
+      <c r="P3" t="str">
+        <f>+'[1]Hoja3 (3)'!$N$2</f>
+        <v>NULL</v>
+      </c>
+      <c r="R3">
+        <f>+'[1]Hoja3 (3)'!$O$2</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" t="str">
+        <f>+'[1]Hoja3 (3)'!$P$2</f>
+        <v>tNO</v>
+      </c>
+      <c r="AC3" t="str">
+        <f>+'[1]Hoja3 (3)'!$Q$2</f>
+        <v>tNO</v>
+      </c>
+      <c r="AD3" t="str">
+        <f>+'[1]Hoja3 (3)'!$R$2</f>
+        <v>tNO</v>
+      </c>
+      <c r="AM3" t="str">
+        <f>+'[1]Hoja3 (3)'!$S$2</f>
+        <v>UND</v>
+      </c>
+      <c r="BA3" t="str">
+        <f>+'[1]Hoja3 (3)'!$T$2</f>
+        <v>UND</v>
+      </c>
+      <c r="CE3" t="str">
+        <f>+'[1]Hoja3 (3)'!$U$2</f>
+        <v>W</v>
+      </c>
+      <c r="CG3">
+        <f>+'[1]Hoja3 (3)'!$V$2</f>
+        <v>0</v>
+      </c>
+      <c r="CH3" t="str">
+        <f>+'[1]Hoja3 (3)'!$W$2</f>
+        <v>tYES</v>
+      </c>
+      <c r="DM3" t="str">
+        <f>+'[1]Hoja3 (3)'!$X$2</f>
+        <v>UND</v>
+      </c>
+      <c r="GS3">
+        <f>+'[1]Hoja3 (3)'!$Y$2</f>
+        <v>1100</v>
+      </c>
+      <c r="GT3">
+        <f>+'[1]Hoja3 (3)'!$Z$2</f>
+        <v>1</v>
+      </c>
+      <c r="GU3">
+        <f>+'[1]Hoja3 (3)'!$AA$2</f>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se van a trabajar actividades pendientes y enviar por correo para el permiso de cargar hoy en la noche 30 de agosto de 2022
</commit_message>
<xml_diff>
--- a/01PlantillaPrueba.xlsx
+++ b/01PlantillaPrueba.xlsx
@@ -1296,11 +1296,11 @@
       <sheetName val="Hoja3 (3)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5">
         <row r="2">
           <cell r="A2" t="str">
@@ -1642,7 +1642,7 @@
   <dimension ref="A1:GU3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="GU4" sqref="GU4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>